<commit_message>
+add version to release
</commit_message>
<xml_diff>
--- a/timeseries_results.xlsx
+++ b/timeseries_results.xlsx
@@ -470,10 +470,10 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -487,10 +487,10 @@
         <v>0.25</v>
       </c>
       <c r="C3" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D3" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
@@ -504,10 +504,10 @@
         <v>0.5</v>
       </c>
       <c r="C4" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D4" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
@@ -521,10 +521,10 @@
         <v>0.75</v>
       </c>
       <c r="C5" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D5" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
@@ -538,10 +538,10 @@
         <v>1</v>
       </c>
       <c r="C6" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
@@ -555,10 +555,10 @@
         <v>1.25</v>
       </c>
       <c r="C7" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D7" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
@@ -572,10 +572,10 @@
         <v>1.5</v>
       </c>
       <c r="C8" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D8" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E8" t="n">
         <v>0</v>
@@ -589,10 +589,10 @@
         <v>1.75</v>
       </c>
       <c r="C9" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D9" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
@@ -623,10 +623,10 @@
         <v>2.25</v>
       </c>
       <c r="C11" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D11" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E11" t="n">
         <v>0</v>
@@ -640,10 +640,10 @@
         <v>2.5</v>
       </c>
       <c r="C12" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D12" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E12" t="n">
         <v>0</v>
@@ -657,10 +657,10 @@
         <v>2.75</v>
       </c>
       <c r="C13" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D13" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
@@ -674,10 +674,10 @@
         <v>3</v>
       </c>
       <c r="C14" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D14" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
@@ -691,10 +691,10 @@
         <v>3.25</v>
       </c>
       <c r="C15" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D15" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E15" t="n">
         <v>0</v>
@@ -725,10 +725,10 @@
         <v>3.75</v>
       </c>
       <c r="C17" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D17" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E17" t="n">
         <v>0</v>
@@ -742,10 +742,10 @@
         <v>4</v>
       </c>
       <c r="C18" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D18" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E18" t="n">
         <v>0</v>
@@ -759,10 +759,10 @@
         <v>4.25</v>
       </c>
       <c r="C19" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D19" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E19" t="n">
         <v>0</v>
@@ -776,10 +776,10 @@
         <v>4.5</v>
       </c>
       <c r="C20" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D20" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E20" t="n">
         <v>0</v>
@@ -810,10 +810,10 @@
         <v>5</v>
       </c>
       <c r="C22" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D22" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E22" t="n">
         <v>0</v>
@@ -827,10 +827,10 @@
         <v>5.25</v>
       </c>
       <c r="C23" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D23" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E23" t="n">
         <v>0</v>
@@ -844,10 +844,10 @@
         <v>5.5</v>
       </c>
       <c r="C24" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D24" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E24" t="n">
         <v>0</v>
@@ -861,10 +861,10 @@
         <v>5.75</v>
       </c>
       <c r="C25" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D25" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E25" t="n">
         <v>0</v>
@@ -878,10 +878,10 @@
         <v>6</v>
       </c>
       <c r="C26" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D26" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E26" t="n">
         <v>0</v>
@@ -895,10 +895,10 @@
         <v>6.25</v>
       </c>
       <c r="C27" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D27" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E27" t="n">
         <v>0</v>
@@ -912,10 +912,10 @@
         <v>6.5</v>
       </c>
       <c r="C28" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D28" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E28" t="n">
         <v>0</v>
@@ -929,10 +929,10 @@
         <v>6.75</v>
       </c>
       <c r="C29" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D29" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E29" t="n">
         <v>0</v>
@@ -946,10 +946,10 @@
         <v>7</v>
       </c>
       <c r="C30" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D30" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E30" t="n">
         <v>0</v>
@@ -963,10 +963,10 @@
         <v>7.25</v>
       </c>
       <c r="C31" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D31" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E31" t="n">
         <v>0</v>
@@ -980,10 +980,10 @@
         <v>7.5</v>
       </c>
       <c r="C32" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="D32" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E32" t="n">
         <v>0</v>
@@ -997,10 +997,10 @@
         <v>7.75</v>
       </c>
       <c r="C33" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D33" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E33" t="n">
         <v>0</v>
@@ -1014,10 +1014,10 @@
         <v>8</v>
       </c>
       <c r="C34" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D34" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E34" t="n">
         <v>0</v>
@@ -1031,10 +1031,10 @@
         <v>8.25</v>
       </c>
       <c r="C35" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D35" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E35" t="n">
         <v>0</v>
@@ -1048,10 +1048,10 @@
         <v>8.5</v>
       </c>
       <c r="C36" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D36" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E36" t="n">
         <v>0</v>
@@ -1065,10 +1065,10 @@
         <v>8.75</v>
       </c>
       <c r="C37" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D37" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E37" t="n">
         <v>0</v>
@@ -1082,10 +1082,10 @@
         <v>9</v>
       </c>
       <c r="C38" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D38" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E38" t="n">
         <v>0</v>
@@ -1099,10 +1099,10 @@
         <v>9.25</v>
       </c>
       <c r="C39" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D39" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E39" t="n">
         <v>0</v>
@@ -1116,10 +1116,10 @@
         <v>9.5</v>
       </c>
       <c r="C40" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D40" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E40" t="n">
         <v>0</v>
@@ -1133,10 +1133,10 @@
         <v>9.75</v>
       </c>
       <c r="C41" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D41" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E41" t="n">
         <v>0</v>
@@ -1150,10 +1150,10 @@
         <v>10</v>
       </c>
       <c r="C42" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D42" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E42" t="n">
         <v>0</v>
@@ -1167,10 +1167,10 @@
         <v>10.25</v>
       </c>
       <c r="C43" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D43" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E43" t="n">
         <v>0</v>
@@ -1201,10 +1201,10 @@
         <v>10.75</v>
       </c>
       <c r="C45" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D45" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E45" t="n">
         <v>0</v>
@@ -1218,10 +1218,10 @@
         <v>11</v>
       </c>
       <c r="C46" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D46" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E46" t="n">
         <v>0</v>
@@ -1235,10 +1235,10 @@
         <v>11.25</v>
       </c>
       <c r="C47" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D47" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E47" t="n">
         <v>0</v>
@@ -1252,10 +1252,10 @@
         <v>11.5</v>
       </c>
       <c r="C48" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D48" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E48" t="n">
         <v>0</v>
@@ -1286,10 +1286,10 @@
         <v>12</v>
       </c>
       <c r="C50" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D50" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E50" t="n">
         <v>0</v>
@@ -1320,10 +1320,10 @@
         <v>12.5</v>
       </c>
       <c r="C52" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D52" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="E52" t="n">
         <v>0</v>
@@ -1337,10 +1337,10 @@
         <v>12.75</v>
       </c>
       <c r="C53" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D53" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E53" t="n">
         <v>0</v>
@@ -1354,13 +1354,13 @@
         <v>13</v>
       </c>
       <c r="C54" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D54" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E54" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="55">
@@ -1371,13 +1371,13 @@
         <v>13.25</v>
       </c>
       <c r="C55" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D55" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E55" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="56">
@@ -1388,13 +1388,13 @@
         <v>13.5</v>
       </c>
       <c r="C56" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D56" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E56" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="57">
@@ -1405,13 +1405,13 @@
         <v>13.75</v>
       </c>
       <c r="C57" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D57" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E57" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="58">
@@ -1422,13 +1422,13 @@
         <v>14</v>
       </c>
       <c r="C58" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D58" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E58" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="59">
@@ -1439,13 +1439,13 @@
         <v>14.25</v>
       </c>
       <c r="C59" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D59" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E59" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60">
@@ -1456,13 +1456,13 @@
         <v>14.5</v>
       </c>
       <c r="C60" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D60" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E60" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61">
@@ -1473,13 +1473,13 @@
         <v>14.75</v>
       </c>
       <c r="C61" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D61" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E61" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="62">
@@ -1490,13 +1490,13 @@
         <v>15</v>
       </c>
       <c r="C62" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D62" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E62" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="63">
@@ -1507,13 +1507,13 @@
         <v>15.25</v>
       </c>
       <c r="C63" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D63" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E63" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="64">
@@ -1524,13 +1524,13 @@
         <v>15.5</v>
       </c>
       <c r="C64" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D64" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E64" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="65">
@@ -1541,13 +1541,13 @@
         <v>15.75</v>
       </c>
       <c r="C65" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D65" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E65" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="66">
@@ -1561,10 +1561,10 @@
         <v>3</v>
       </c>
       <c r="D66" t="n">
+        <v>0</v>
+      </c>
+      <c r="E66" t="n">
         <v>3</v>
-      </c>
-      <c r="E66" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="67">
@@ -1575,13 +1575,13 @@
         <v>16.25</v>
       </c>
       <c r="C67" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D67" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E67" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="68">
@@ -1592,13 +1592,13 @@
         <v>16.5</v>
       </c>
       <c r="C68" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D68" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E68" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="69">
@@ -1609,13 +1609,13 @@
         <v>16.75</v>
       </c>
       <c r="C69" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D69" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E69" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="70">
@@ -1626,13 +1626,13 @@
         <v>17</v>
       </c>
       <c r="C70" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D70" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E70" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="71">
@@ -1643,13 +1643,13 @@
         <v>17.25</v>
       </c>
       <c r="C71" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D71" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E71" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="72">
@@ -1663,10 +1663,10 @@
         <v>7</v>
       </c>
       <c r="D72" t="n">
+        <v>0</v>
+      </c>
+      <c r="E72" t="n">
         <v>7</v>
-      </c>
-      <c r="E72" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="73">
@@ -1677,13 +1677,13 @@
         <v>17.75</v>
       </c>
       <c r="C73" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D73" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E73" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="74">
@@ -1694,13 +1694,13 @@
         <v>18</v>
       </c>
       <c r="C74" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D74" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E74" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="75">
@@ -1711,13 +1711,13 @@
         <v>18.25</v>
       </c>
       <c r="C75" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="D75" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E75" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76">
@@ -1728,13 +1728,13 @@
         <v>18.5</v>
       </c>
       <c r="C76" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D76" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E76" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="77">
@@ -1745,13 +1745,13 @@
         <v>18.75</v>
       </c>
       <c r="C77" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D77" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E77" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="78">
@@ -1762,13 +1762,13 @@
         <v>19</v>
       </c>
       <c r="C78" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D78" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E78" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79">
@@ -1779,13 +1779,13 @@
         <v>19.25</v>
       </c>
       <c r="C79" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D79" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E79" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="80">
@@ -1796,13 +1796,13 @@
         <v>19.5</v>
       </c>
       <c r="C80" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D80" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E80" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="81">
@@ -1813,13 +1813,13 @@
         <v>19.75</v>
       </c>
       <c r="C81" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D81" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E81" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="82">
@@ -1830,13 +1830,13 @@
         <v>20</v>
       </c>
       <c r="C82" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D82" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E82" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="83">
@@ -1847,13 +1847,13 @@
         <v>20.25</v>
       </c>
       <c r="C83" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D83" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E83" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="84">
@@ -1864,13 +1864,13 @@
         <v>20.5</v>
       </c>
       <c r="C84" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D84" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E84" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="85">
@@ -1881,13 +1881,13 @@
         <v>20.75</v>
       </c>
       <c r="C85" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D85" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E85" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="86">
@@ -1898,13 +1898,13 @@
         <v>21</v>
       </c>
       <c r="C86" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D86" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E86" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="87">
@@ -1915,13 +1915,13 @@
         <v>21.25</v>
       </c>
       <c r="C87" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D87" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E87" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="88">
@@ -1932,13 +1932,13 @@
         <v>21.5</v>
       </c>
       <c r="C88" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D88" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E88" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="89">
@@ -1952,10 +1952,10 @@
         <v>4</v>
       </c>
       <c r="D89" t="n">
+        <v>0</v>
+      </c>
+      <c r="E89" t="n">
         <v>4</v>
-      </c>
-      <c r="E89" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="90">
@@ -1969,10 +1969,10 @@
         <v>2</v>
       </c>
       <c r="D90" t="n">
+        <v>0</v>
+      </c>
+      <c r="E90" t="n">
         <v>2</v>
-      </c>
-      <c r="E90" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="91">
@@ -1986,10 +1986,10 @@
         <v>5</v>
       </c>
       <c r="D91" t="n">
+        <v>0</v>
+      </c>
+      <c r="E91" t="n">
         <v>5</v>
-      </c>
-      <c r="E91" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="92">
@@ -2000,13 +2000,13 @@
         <v>22.5</v>
       </c>
       <c r="C92" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D92" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E92" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="93">
@@ -2020,10 +2020,10 @@
         <v>7</v>
       </c>
       <c r="D93" t="n">
+        <v>0</v>
+      </c>
+      <c r="E93" t="n">
         <v>7</v>
-      </c>
-      <c r="E93" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="94">
@@ -2034,13 +2034,13 @@
         <v>23</v>
       </c>
       <c r="C94" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D94" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E94" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="95">
@@ -2051,13 +2051,13 @@
         <v>23.25</v>
       </c>
       <c r="C95" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D95" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E95" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="96">
@@ -2068,13 +2068,13 @@
         <v>23.5</v>
       </c>
       <c r="C96" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D96" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E96" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="97">
@@ -2085,13 +2085,13 @@
         <v>23.75</v>
       </c>
       <c r="C97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D97" t="n">
         <v>0</v>
       </c>
       <c r="E97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2710,7 +2710,7 @@
         <v>13</v>
       </c>
       <c r="C54" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="55">
@@ -2721,7 +2721,7 @@
         <v>13.25</v>
       </c>
       <c r="C55" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="56">
@@ -2732,7 +2732,7 @@
         <v>13.5</v>
       </c>
       <c r="C56" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="57">
@@ -2743,7 +2743,7 @@
         <v>13.75</v>
       </c>
       <c r="C57" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="58">
@@ -2754,7 +2754,7 @@
         <v>14</v>
       </c>
       <c r="C58" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="59">
@@ -2765,7 +2765,7 @@
         <v>14.25</v>
       </c>
       <c r="C59" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60">
@@ -2776,7 +2776,7 @@
         <v>14.5</v>
       </c>
       <c r="C60" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61">
@@ -2787,7 +2787,7 @@
         <v>14.75</v>
       </c>
       <c r="C61" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="62">
@@ -2798,7 +2798,7 @@
         <v>15</v>
       </c>
       <c r="C62" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="63">
@@ -2809,7 +2809,7 @@
         <v>15.25</v>
       </c>
       <c r="C63" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="64">
@@ -2820,7 +2820,7 @@
         <v>15.5</v>
       </c>
       <c r="C64" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="65">
@@ -2831,7 +2831,7 @@
         <v>15.75</v>
       </c>
       <c r="C65" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="66">
@@ -2842,7 +2842,7 @@
         <v>16</v>
       </c>
       <c r="C66" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="67">
@@ -2853,7 +2853,7 @@
         <v>16.25</v>
       </c>
       <c r="C67" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="68">
@@ -2864,7 +2864,7 @@
         <v>16.5</v>
       </c>
       <c r="C68" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="69">
@@ -2875,7 +2875,7 @@
         <v>16.75</v>
       </c>
       <c r="C69" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="70">
@@ -2886,7 +2886,7 @@
         <v>17</v>
       </c>
       <c r="C70" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="71">
@@ -2897,7 +2897,7 @@
         <v>17.25</v>
       </c>
       <c r="C71" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="72">
@@ -2908,7 +2908,7 @@
         <v>17.5</v>
       </c>
       <c r="C72" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="73">
@@ -2919,7 +2919,7 @@
         <v>17.75</v>
       </c>
       <c r="C73" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="74">
@@ -2930,7 +2930,7 @@
         <v>18</v>
       </c>
       <c r="C74" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="75">
@@ -2941,7 +2941,7 @@
         <v>18.25</v>
       </c>
       <c r="C75" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76">
@@ -2952,7 +2952,7 @@
         <v>18.5</v>
       </c>
       <c r="C76" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="77">
@@ -2963,7 +2963,7 @@
         <v>18.75</v>
       </c>
       <c r="C77" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="78">
@@ -2974,7 +2974,7 @@
         <v>19</v>
       </c>
       <c r="C78" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79">
@@ -2985,7 +2985,7 @@
         <v>19.25</v>
       </c>
       <c r="C79" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="80">
@@ -2996,7 +2996,7 @@
         <v>19.5</v>
       </c>
       <c r="C80" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="81">
@@ -3007,7 +3007,7 @@
         <v>19.75</v>
       </c>
       <c r="C81" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="82">
@@ -3018,7 +3018,7 @@
         <v>20</v>
       </c>
       <c r="C82" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="83">
@@ -3029,7 +3029,7 @@
         <v>20.25</v>
       </c>
       <c r="C83" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="84">
@@ -3040,7 +3040,7 @@
         <v>20.5</v>
       </c>
       <c r="C84" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="85">
@@ -3051,7 +3051,7 @@
         <v>20.75</v>
       </c>
       <c r="C85" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="86">
@@ -3062,7 +3062,7 @@
         <v>21</v>
       </c>
       <c r="C86" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="87">
@@ -3073,7 +3073,7 @@
         <v>21.25</v>
       </c>
       <c r="C87" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="88">
@@ -3084,7 +3084,7 @@
         <v>21.5</v>
       </c>
       <c r="C88" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="89">
@@ -3095,7 +3095,7 @@
         <v>21.75</v>
       </c>
       <c r="C89" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="90">
@@ -3106,7 +3106,7 @@
         <v>22</v>
       </c>
       <c r="C90" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="91">
@@ -3117,7 +3117,7 @@
         <v>22.25</v>
       </c>
       <c r="C91" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="92">
@@ -3128,7 +3128,7 @@
         <v>22.5</v>
       </c>
       <c r="C92" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="93">
@@ -3139,7 +3139,7 @@
         <v>22.75</v>
       </c>
       <c r="C93" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="94">
@@ -3150,7 +3150,7 @@
         <v>23</v>
       </c>
       <c r="C94" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="95">
@@ -3161,7 +3161,7 @@
         <v>23.25</v>
       </c>
       <c r="C95" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="96">
@@ -3172,7 +3172,7 @@
         <v>23.5</v>
       </c>
       <c r="C96" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="97">
@@ -3183,7 +3183,7 @@
         <v>23.75</v>
       </c>
       <c r="C97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -3240,13 +3240,13 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>348</v>
+        <v>8</v>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E2" t="n">
-        <v>0.002873563218390805</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -3257,13 +3257,13 @@
         <v>0.25</v>
       </c>
       <c r="C3" t="n">
-        <v>402</v>
+        <v>2</v>
       </c>
       <c r="D3" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E3" t="n">
-        <v>0.009950248756218905</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -3274,13 +3274,13 @@
         <v>0.5</v>
       </c>
       <c r="C4" t="n">
-        <v>408</v>
+        <v>5</v>
       </c>
       <c r="D4" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E4" t="n">
-        <v>0.0196078431372549</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -3291,13 +3291,13 @@
         <v>0.75</v>
       </c>
       <c r="C5" t="n">
-        <v>408</v>
+        <v>10</v>
       </c>
       <c r="D5" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>0.01715686274509804</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -3308,13 +3308,13 @@
         <v>1</v>
       </c>
       <c r="C6" t="n">
-        <v>408</v>
+        <v>9</v>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E6" t="n">
-        <v>0.002450980392156863</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -3325,13 +3325,13 @@
         <v>1.25</v>
       </c>
       <c r="C7" t="n">
-        <v>420</v>
+        <v>1</v>
       </c>
       <c r="D7" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E7" t="n">
-        <v>0.009523809523809525</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
@@ -3342,13 +3342,13 @@
         <v>1.5</v>
       </c>
       <c r="C8" t="n">
-        <v>420</v>
+        <v>4</v>
       </c>
       <c r="D8" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E8" t="n">
-        <v>0.01666666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
@@ -3359,13 +3359,13 @@
         <v>1.75</v>
       </c>
       <c r="C9" t="n">
-        <v>420</v>
+        <v>3</v>
       </c>
       <c r="D9" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E9" t="n">
-        <v>0.01666666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
@@ -3376,13 +3376,13 @@
         <v>2</v>
       </c>
       <c r="C10" t="n">
-        <v>420</v>
+        <v>1</v>
       </c>
       <c r="D10" t="n">
         <v>1</v>
       </c>
       <c r="E10" t="n">
-        <v>0.002380952380952381</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
@@ -3393,13 +3393,13 @@
         <v>2.25</v>
       </c>
       <c r="C11" t="n">
-        <v>420</v>
+        <v>3</v>
       </c>
       <c r="D11" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E11" t="n">
-        <v>0.01428571428571429</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
@@ -3410,13 +3410,13 @@
         <v>2.5</v>
       </c>
       <c r="C12" t="n">
-        <v>426</v>
+        <v>9</v>
       </c>
       <c r="D12" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E12" t="n">
-        <v>0.002347417840375587</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
@@ -3427,13 +3427,13 @@
         <v>2.75</v>
       </c>
       <c r="C13" t="n">
-        <v>432</v>
+        <v>8</v>
       </c>
       <c r="D13" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E13" t="n">
-        <v>0.02083333333333333</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
@@ -3444,13 +3444,13 @@
         <v>3</v>
       </c>
       <c r="C14" t="n">
-        <v>438</v>
+        <v>9</v>
       </c>
       <c r="D14" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E14" t="n">
-        <v>0.0136986301369863</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15">
@@ -3461,13 +3461,13 @@
         <v>3.25</v>
       </c>
       <c r="C15" t="n">
-        <v>438</v>
+        <v>10</v>
       </c>
       <c r="D15" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E15" t="n">
-        <v>0.0091324200913242</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16">
@@ -3478,13 +3478,13 @@
         <v>3.5</v>
       </c>
       <c r="C16" t="n">
-        <v>444</v>
+        <v>6</v>
       </c>
       <c r="D16" t="n">
         <v>6</v>
       </c>
       <c r="E16" t="n">
-        <v>0.01351351351351351</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
@@ -3495,13 +3495,13 @@
         <v>3.75</v>
       </c>
       <c r="C17" t="n">
-        <v>444</v>
+        <v>10</v>
       </c>
       <c r="D17" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>0.01126126126126126</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
@@ -3512,13 +3512,13 @@
         <v>4</v>
       </c>
       <c r="C18" t="n">
-        <v>444</v>
+        <v>2</v>
       </c>
       <c r="D18" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E18" t="n">
-        <v>0.02252252252252252</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19">
@@ -3529,13 +3529,13 @@
         <v>4.25</v>
       </c>
       <c r="C19" t="n">
-        <v>444</v>
+        <v>2</v>
       </c>
       <c r="D19" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E19" t="n">
-        <v>0.02252252252252252</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20">
@@ -3546,13 +3546,13 @@
         <v>4.5</v>
       </c>
       <c r="C20" t="n">
-        <v>444</v>
+        <v>10</v>
       </c>
       <c r="D20" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>0.01351351351351351</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21">
@@ -3563,13 +3563,13 @@
         <v>4.75</v>
       </c>
       <c r="C21" t="n">
-        <v>450</v>
+        <v>6</v>
       </c>
       <c r="D21" t="n">
         <v>6</v>
       </c>
       <c r="E21" t="n">
-        <v>0.01333333333333333</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22">
@@ -3580,13 +3580,13 @@
         <v>5</v>
       </c>
       <c r="C22" t="n">
-        <v>456</v>
+        <v>2</v>
       </c>
       <c r="D22" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E22" t="n">
-        <v>0.01535087719298246</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23">
@@ -3597,13 +3597,13 @@
         <v>5.25</v>
       </c>
       <c r="C23" t="n">
-        <v>456</v>
+        <v>5</v>
       </c>
       <c r="D23" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E23" t="n">
-        <v>0.004385964912280702</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24">
@@ -3614,13 +3614,13 @@
         <v>5.5</v>
       </c>
       <c r="C24" t="n">
-        <v>456</v>
+        <v>10</v>
       </c>
       <c r="D24" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>0.006578947368421052</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25">
@@ -3631,13 +3631,13 @@
         <v>5.75</v>
       </c>
       <c r="C25" t="n">
-        <v>462</v>
+        <v>4</v>
       </c>
       <c r="D25" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E25" t="n">
-        <v>0.006493506493506494</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26">
@@ -3648,13 +3648,13 @@
         <v>6</v>
       </c>
       <c r="C26" t="n">
-        <v>462</v>
+        <v>3</v>
       </c>
       <c r="D26" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E26" t="n">
-        <v>0.02164502164502164</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27">
@@ -3665,13 +3665,13 @@
         <v>6.25</v>
       </c>
       <c r="C27" t="n">
-        <v>462</v>
+        <v>6</v>
       </c>
       <c r="D27" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E27" t="n">
-        <v>0.02164502164502164</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28">
@@ -3682,13 +3682,13 @@
         <v>6.5</v>
       </c>
       <c r="C28" t="n">
-        <v>462</v>
+        <v>2</v>
       </c>
       <c r="D28" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E28" t="n">
-        <v>0.02164502164502164</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29">
@@ -3699,13 +3699,13 @@
         <v>6.75</v>
       </c>
       <c r="C29" t="n">
-        <v>462</v>
+        <v>3</v>
       </c>
       <c r="D29" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E29" t="n">
-        <v>0.01082251082251082</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30">
@@ -3716,13 +3716,13 @@
         <v>7</v>
       </c>
       <c r="C30" t="n">
-        <v>462</v>
+        <v>7</v>
       </c>
       <c r="D30" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E30" t="n">
-        <v>0.006493506493506494</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31">
@@ -3733,13 +3733,13 @@
         <v>7.25</v>
       </c>
       <c r="C31" t="n">
-        <v>480</v>
+        <v>3</v>
       </c>
       <c r="D31" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E31" t="n">
-        <v>0.02083333333333333</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32">
@@ -3750,13 +3750,13 @@
         <v>7.5</v>
       </c>
       <c r="C32" t="n">
-        <v>492</v>
+        <v>1</v>
       </c>
       <c r="D32" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E32" t="n">
-        <v>0.01829268292682927</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33">
@@ -3767,13 +3767,13 @@
         <v>7.75</v>
       </c>
       <c r="C33" t="n">
-        <v>498</v>
+        <v>6</v>
       </c>
       <c r="D33" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E33" t="n">
-        <v>0.01606425702811245</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34">
@@ -3784,13 +3784,13 @@
         <v>8</v>
       </c>
       <c r="C34" t="n">
-        <v>510</v>
+        <v>6</v>
       </c>
       <c r="D34" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E34" t="n">
-        <v>0.01372549019607843</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35">
@@ -3801,13 +3801,13 @@
         <v>8.25</v>
       </c>
       <c r="C35" t="n">
-        <v>516</v>
+        <v>8</v>
       </c>
       <c r="D35" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E35" t="n">
-        <v>0.01744186046511628</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36">
@@ -3818,13 +3818,13 @@
         <v>8.5</v>
       </c>
       <c r="C36" t="n">
-        <v>528</v>
+        <v>10</v>
       </c>
       <c r="D36" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E36" t="n">
-        <v>0.01136363636363636</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37">
@@ -3835,13 +3835,13 @@
         <v>8.75</v>
       </c>
       <c r="C37" t="n">
-        <v>534</v>
+        <v>9</v>
       </c>
       <c r="D37" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E37" t="n">
-        <v>0.01872659176029963</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38">
@@ -3852,13 +3852,13 @@
         <v>9</v>
       </c>
       <c r="C38" t="n">
-        <v>540</v>
+        <v>3</v>
       </c>
       <c r="D38" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E38" t="n">
-        <v>0.01111111111111111</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39">
@@ -3869,13 +3869,13 @@
         <v>9.25</v>
       </c>
       <c r="C39" t="n">
-        <v>270</v>
+        <v>9</v>
       </c>
       <c r="D39" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E39" t="n">
-        <v>0.02962962962962963</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40">
@@ -3886,13 +3886,13 @@
         <v>9.5</v>
       </c>
       <c r="C40" t="n">
-        <v>246</v>
+        <v>3</v>
       </c>
       <c r="D40" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E40" t="n">
-        <v>0.008130081300813009</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41">
@@ -3903,13 +3903,13 @@
         <v>9.75</v>
       </c>
       <c r="C41" t="n">
-        <v>246</v>
+        <v>4</v>
       </c>
       <c r="D41" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E41" t="n">
-        <v>0.03252032520325204</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42">
@@ -3920,13 +3920,13 @@
         <v>10</v>
       </c>
       <c r="C42" t="n">
-        <v>240</v>
+        <v>6</v>
       </c>
       <c r="D42" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E42" t="n">
-        <v>0.0125</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43">
@@ -3937,13 +3937,13 @@
         <v>10.25</v>
       </c>
       <c r="C43" t="n">
-        <v>246</v>
+        <v>3</v>
       </c>
       <c r="D43" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E43" t="n">
-        <v>0.01626016260162602</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44">
@@ -3954,13 +3954,13 @@
         <v>10.5</v>
       </c>
       <c r="C44" t="n">
-        <v>240</v>
+        <v>5</v>
       </c>
       <c r="D44" t="n">
         <v>5</v>
       </c>
       <c r="E44" t="n">
-        <v>0.02083333333333333</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45">
@@ -3971,13 +3971,13 @@
         <v>10.75</v>
       </c>
       <c r="C45" t="n">
-        <v>246</v>
+        <v>9</v>
       </c>
       <c r="D45" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E45" t="n">
-        <v>0.02439024390243903</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46">
@@ -3988,13 +3988,13 @@
         <v>11</v>
       </c>
       <c r="C46" t="n">
-        <v>240</v>
+        <v>8</v>
       </c>
       <c r="D46" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E46" t="n">
-        <v>0.025</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47">
@@ -4005,13 +4005,13 @@
         <v>11.25</v>
       </c>
       <c r="C47" t="n">
-        <v>240</v>
+        <v>6</v>
       </c>
       <c r="D47" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E47" t="n">
-        <v>0.0125</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48">
@@ -4022,13 +4022,13 @@
         <v>11.5</v>
       </c>
       <c r="C48" t="n">
-        <v>246</v>
+        <v>6</v>
       </c>
       <c r="D48" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E48" t="n">
-        <v>0.01219512195121951</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49">
@@ -4039,13 +4039,13 @@
         <v>11.75</v>
       </c>
       <c r="C49" t="n">
-        <v>252</v>
+        <v>6</v>
       </c>
       <c r="D49" t="n">
         <v>6</v>
       </c>
       <c r="E49" t="n">
-        <v>0.02380952380952381</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50">
@@ -4056,13 +4056,13 @@
         <v>12</v>
       </c>
       <c r="C50" t="n">
-        <v>246</v>
+        <v>6</v>
       </c>
       <c r="D50" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E50" t="n">
-        <v>0.008130081300813009</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51">
@@ -4073,13 +4073,13 @@
         <v>12.25</v>
       </c>
       <c r="C51" t="n">
-        <v>246</v>
+        <v>8</v>
       </c>
       <c r="D51" t="n">
         <v>8</v>
       </c>
       <c r="E51" t="n">
-        <v>0.03252032520325204</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52">
@@ -4090,13 +4090,13 @@
         <v>12.5</v>
       </c>
       <c r="C52" t="n">
-        <v>240</v>
+        <v>9</v>
       </c>
       <c r="D52" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="E52" t="n">
-        <v>0.008333333333333333</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53">
@@ -4107,13 +4107,13 @@
         <v>12.75</v>
       </c>
       <c r="C53" t="n">
-        <v>228</v>
+        <v>10</v>
       </c>
       <c r="D53" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>0.0131578947368421</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54">
@@ -4124,13 +4124,13 @@
         <v>13</v>
       </c>
       <c r="C54" t="n">
-        <v>234</v>
+        <v>0</v>
       </c>
       <c r="D54" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E54" t="n">
-        <v>0.02564102564102564</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55">
@@ -4141,13 +4141,13 @@
         <v>13.25</v>
       </c>
       <c r="C55" t="n">
-        <v>234</v>
+        <v>0</v>
       </c>
       <c r="D55" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E55" t="n">
-        <v>0.01282051282051282</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56">
@@ -4158,13 +4158,13 @@
         <v>13.5</v>
       </c>
       <c r="C56" t="n">
-        <v>252</v>
+        <v>0</v>
       </c>
       <c r="D56" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E56" t="n">
-        <v>0.02380952380952381</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57">
@@ -4175,13 +4175,13 @@
         <v>13.75</v>
       </c>
       <c r="C57" t="n">
-        <v>258</v>
+        <v>0</v>
       </c>
       <c r="D57" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E57" t="n">
-        <v>0.03488372093023256</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58">
@@ -4192,13 +4192,13 @@
         <v>14</v>
       </c>
       <c r="C58" t="n">
-        <v>258</v>
+        <v>0</v>
       </c>
       <c r="D58" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E58" t="n">
-        <v>0.01162790697674419</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59">
@@ -4209,13 +4209,13 @@
         <v>14.25</v>
       </c>
       <c r="C59" t="n">
-        <v>270</v>
+        <v>0</v>
       </c>
       <c r="D59" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E59" t="n">
-        <v>0.01481481481481482</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60">
@@ -4226,13 +4226,13 @@
         <v>14.5</v>
       </c>
       <c r="C60" t="n">
-        <v>294</v>
+        <v>0</v>
       </c>
       <c r="D60" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E60" t="n">
-        <v>0.02040816326530612</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61">
@@ -4243,13 +4243,13 @@
         <v>14.75</v>
       </c>
       <c r="C61" t="n">
-        <v>294</v>
+        <v>0</v>
       </c>
       <c r="D61" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E61" t="n">
-        <v>0.0272108843537415</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62">
@@ -4260,13 +4260,13 @@
         <v>15</v>
       </c>
       <c r="C62" t="n">
-        <v>276</v>
+        <v>0</v>
       </c>
       <c r="D62" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E62" t="n">
-        <v>0.02536231884057971</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63">
@@ -4277,13 +4277,13 @@
         <v>15.25</v>
       </c>
       <c r="C63" t="n">
-        <v>270</v>
+        <v>0</v>
       </c>
       <c r="D63" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E63" t="n">
-        <v>0.01111111111111111</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64">
@@ -4294,13 +4294,13 @@
         <v>15.5</v>
       </c>
       <c r="C64" t="n">
-        <v>264</v>
+        <v>0</v>
       </c>
       <c r="D64" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E64" t="n">
-        <v>0.02651515151515152</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65">
@@ -4311,13 +4311,13 @@
         <v>15.75</v>
       </c>
       <c r="C65" t="n">
-        <v>264</v>
+        <v>0</v>
       </c>
       <c r="D65" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E65" t="n">
-        <v>0.01136363636363636</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66">
@@ -4328,13 +4328,13 @@
         <v>16</v>
       </c>
       <c r="C66" t="n">
-        <v>258</v>
+        <v>0</v>
       </c>
       <c r="D66" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E66" t="n">
-        <v>0.01162790697674419</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67">
@@ -4345,13 +4345,13 @@
         <v>16.25</v>
       </c>
       <c r="C67" t="n">
-        <v>252</v>
+        <v>0</v>
       </c>
       <c r="D67" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E67" t="n">
-        <v>0.03571428571428571</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68">
@@ -4362,13 +4362,13 @@
         <v>16.5</v>
       </c>
       <c r="C68" t="n">
-        <v>246</v>
+        <v>0</v>
       </c>
       <c r="D68" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E68" t="n">
-        <v>0.02845528455284553</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69">
@@ -4379,13 +4379,13 @@
         <v>16.75</v>
       </c>
       <c r="C69" t="n">
-        <v>240</v>
+        <v>0</v>
       </c>
       <c r="D69" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E69" t="n">
-        <v>0.04166666666666666</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70">
@@ -4396,13 +4396,13 @@
         <v>17</v>
       </c>
       <c r="C70" t="n">
-        <v>234</v>
+        <v>0</v>
       </c>
       <c r="D70" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E70" t="n">
-        <v>0.02564102564102564</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71">
@@ -4413,13 +4413,13 @@
         <v>17.25</v>
       </c>
       <c r="C71" t="n">
-        <v>234</v>
+        <v>0</v>
       </c>
       <c r="D71" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E71" t="n">
-        <v>0.03418803418803419</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72">
@@ -4430,13 +4430,13 @@
         <v>17.5</v>
       </c>
       <c r="C72" t="n">
-        <v>228</v>
+        <v>0</v>
       </c>
       <c r="D72" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E72" t="n">
-        <v>0.03070175438596491</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73">
@@ -4447,13 +4447,13 @@
         <v>17.75</v>
       </c>
       <c r="C73" t="n">
-        <v>228</v>
+        <v>0</v>
       </c>
       <c r="D73" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E73" t="n">
-        <v>0.02192982456140351</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74">
@@ -4464,13 +4464,13 @@
         <v>18</v>
       </c>
       <c r="C74" t="n">
-        <v>210</v>
+        <v>0</v>
       </c>
       <c r="D74" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E74" t="n">
-        <v>0.0380952380952381</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75">
@@ -4481,13 +4481,13 @@
         <v>18.25</v>
       </c>
       <c r="C75" t="n">
-        <v>198</v>
+        <v>0</v>
       </c>
       <c r="D75" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E75" t="n">
-        <v>0.04545454545454546</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76">
@@ -4498,13 +4498,13 @@
         <v>18.5</v>
       </c>
       <c r="C76" t="n">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="D76" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E76" t="n">
-        <v>0.03888888888888889</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77">
@@ -4515,13 +4515,13 @@
         <v>18.75</v>
       </c>
       <c r="C77" t="n">
-        <v>174</v>
+        <v>0</v>
       </c>
       <c r="D77" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E77" t="n">
-        <v>0.005747126436781609</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78">
@@ -4532,13 +4532,13 @@
         <v>19</v>
       </c>
       <c r="C78" t="n">
-        <v>174</v>
+        <v>0</v>
       </c>
       <c r="D78" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E78" t="n">
-        <v>0.01149425287356322</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79">
@@ -4549,13 +4549,13 @@
         <v>19.25</v>
       </c>
       <c r="C79" t="n">
-        <v>168</v>
+        <v>0</v>
       </c>
       <c r="D79" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E79" t="n">
-        <v>0.02976190476190476</v>
+        <v>0</v>
       </c>
     </row>
     <row r="80">
@@ -4566,13 +4566,13 @@
         <v>19.5</v>
       </c>
       <c r="C80" t="n">
-        <v>162</v>
+        <v>0</v>
       </c>
       <c r="D80" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E80" t="n">
-        <v>0.05555555555555555</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81">
@@ -4583,13 +4583,13 @@
         <v>19.75</v>
       </c>
       <c r="C81" t="n">
-        <v>162</v>
+        <v>0</v>
       </c>
       <c r="D81" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E81" t="n">
-        <v>0.0308641975308642</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82">
@@ -4600,13 +4600,13 @@
         <v>20</v>
       </c>
       <c r="C82" t="n">
-        <v>156</v>
+        <v>0</v>
       </c>
       <c r="D82" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E82" t="n">
-        <v>0.0576923076923077</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83">
@@ -4617,13 +4617,13 @@
         <v>20.25</v>
       </c>
       <c r="C83" t="n">
-        <v>138</v>
+        <v>0</v>
       </c>
       <c r="D83" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E83" t="n">
-        <v>0.05797101449275362</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84">
@@ -4634,13 +4634,13 @@
         <v>20.5</v>
       </c>
       <c r="C84" t="n">
-        <v>138</v>
+        <v>0</v>
       </c>
       <c r="D84" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E84" t="n">
-        <v>0.007246376811594203</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85">
@@ -4651,13 +4651,13 @@
         <v>20.75</v>
       </c>
       <c r="C85" t="n">
-        <v>126</v>
+        <v>0</v>
       </c>
       <c r="D85" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E85" t="n">
-        <v>0.03174603174603174</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86">
@@ -4668,13 +4668,13 @@
         <v>21</v>
       </c>
       <c r="C86" t="n">
-        <v>126</v>
+        <v>0</v>
       </c>
       <c r="D86" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E86" t="n">
-        <v>0.03174603174603174</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87">
@@ -4685,13 +4685,13 @@
         <v>21.25</v>
       </c>
       <c r="C87" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="D87" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E87" t="n">
-        <v>0.008333333333333333</v>
+        <v>0</v>
       </c>
     </row>
     <row r="88">
@@ -4702,13 +4702,13 @@
         <v>21.5</v>
       </c>
       <c r="C88" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="D88" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E88" t="n">
-        <v>0.03333333333333333</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89">
@@ -4719,13 +4719,13 @@
         <v>21.75</v>
       </c>
       <c r="C89" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="D89" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E89" t="n">
-        <v>0.03333333333333333</v>
+        <v>0</v>
       </c>
     </row>
     <row r="90">
@@ -4736,13 +4736,13 @@
         <v>22</v>
       </c>
       <c r="C90" t="n">
-        <v>114</v>
+        <v>0</v>
       </c>
       <c r="D90" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E90" t="n">
-        <v>0.01754385964912281</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91">
@@ -4753,13 +4753,13 @@
         <v>22.25</v>
       </c>
       <c r="C91" t="n">
-        <v>114</v>
+        <v>0</v>
       </c>
       <c r="D91" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E91" t="n">
-        <v>0.04385964912280702</v>
+        <v>0</v>
       </c>
     </row>
     <row r="92">
@@ -4770,13 +4770,13 @@
         <v>22.5</v>
       </c>
       <c r="C92" t="n">
-        <v>102</v>
+        <v>0</v>
       </c>
       <c r="D92" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E92" t="n">
-        <v>0.05882352941176471</v>
+        <v>0</v>
       </c>
     </row>
     <row r="93">
@@ -4787,13 +4787,13 @@
         <v>22.75</v>
       </c>
       <c r="C93" t="n">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="D93" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E93" t="n">
-        <v>0.07777777777777778</v>
+        <v>0</v>
       </c>
     </row>
     <row r="94">
@@ -4804,13 +4804,13 @@
         <v>23</v>
       </c>
       <c r="C94" t="n">
-        <v>84</v>
+        <v>0</v>
       </c>
       <c r="D94" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E94" t="n">
-        <v>0.05952380952380952</v>
+        <v>0</v>
       </c>
     </row>
     <row r="95">
@@ -4821,13 +4821,13 @@
         <v>23.25</v>
       </c>
       <c r="C95" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="D95" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E95" t="n">
-        <v>0.05555555555555555</v>
+        <v>0</v>
       </c>
     </row>
     <row r="96">
@@ -4838,13 +4838,13 @@
         <v>23.5</v>
       </c>
       <c r="C96" t="n">
-        <v>66</v>
+        <v>0</v>
       </c>
       <c r="D96" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E96" t="n">
-        <v>0.01515151515151515</v>
+        <v>0</v>
       </c>
     </row>
     <row r="97">

</xml_diff>

<commit_message>
feat: initialize core application structure, add thesis document files, and update timeseries results.
</commit_message>
<xml_diff>
--- a/timeseries_results.xlsx
+++ b/timeseries_results.xlsx
@@ -470,10 +470,10 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D2" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -487,10 +487,10 @@
         <v>0.25</v>
       </c>
       <c r="C3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
@@ -504,10 +504,10 @@
         <v>0.5</v>
       </c>
       <c r="C4" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D4" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
@@ -555,10 +555,10 @@
         <v>1.25</v>
       </c>
       <c r="C7" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
@@ -572,10 +572,10 @@
         <v>1.5</v>
       </c>
       <c r="C8" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D8" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E8" t="n">
         <v>0</v>
@@ -606,10 +606,10 @@
         <v>2</v>
       </c>
       <c r="C10" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D10" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
@@ -623,10 +623,10 @@
         <v>2.25</v>
       </c>
       <c r="C11" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D11" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E11" t="n">
         <v>0</v>
@@ -640,10 +640,10 @@
         <v>2.5</v>
       </c>
       <c r="C12" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="D12" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E12" t="n">
         <v>0</v>
@@ -674,10 +674,10 @@
         <v>3</v>
       </c>
       <c r="C14" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="D14" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
@@ -691,10 +691,10 @@
         <v>3.25</v>
       </c>
       <c r="C15" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D15" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E15" t="n">
         <v>0</v>
@@ -708,10 +708,10 @@
         <v>3.5</v>
       </c>
       <c r="C16" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D16" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E16" t="n">
         <v>0</v>
@@ -725,10 +725,10 @@
         <v>3.75</v>
       </c>
       <c r="C17" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D17" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E17" t="n">
         <v>0</v>
@@ -759,10 +759,10 @@
         <v>4.25</v>
       </c>
       <c r="C19" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D19" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E19" t="n">
         <v>0</v>
@@ -776,10 +776,10 @@
         <v>4.5</v>
       </c>
       <c r="C20" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D20" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E20" t="n">
         <v>0</v>
@@ -793,10 +793,10 @@
         <v>4.75</v>
       </c>
       <c r="C21" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D21" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E21" t="n">
         <v>0</v>
@@ -810,10 +810,10 @@
         <v>5</v>
       </c>
       <c r="C22" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D22" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="E22" t="n">
         <v>0</v>
@@ -827,10 +827,10 @@
         <v>5.25</v>
       </c>
       <c r="C23" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D23" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E23" t="n">
         <v>0</v>
@@ -844,10 +844,10 @@
         <v>5.5</v>
       </c>
       <c r="C24" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D24" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E24" t="n">
         <v>0</v>
@@ -861,10 +861,10 @@
         <v>5.75</v>
       </c>
       <c r="C25" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D25" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E25" t="n">
         <v>0</v>
@@ -878,10 +878,10 @@
         <v>6</v>
       </c>
       <c r="C26" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D26" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E26" t="n">
         <v>0</v>
@@ -895,10 +895,10 @@
         <v>6.25</v>
       </c>
       <c r="C27" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D27" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E27" t="n">
         <v>0</v>
@@ -912,10 +912,10 @@
         <v>6.5</v>
       </c>
       <c r="C28" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D28" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E28" t="n">
         <v>0</v>
@@ -929,10 +929,10 @@
         <v>6.75</v>
       </c>
       <c r="C29" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D29" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E29" t="n">
         <v>0</v>
@@ -946,10 +946,10 @@
         <v>7</v>
       </c>
       <c r="C30" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D30" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E30" t="n">
         <v>0</v>
@@ -980,10 +980,10 @@
         <v>7.5</v>
       </c>
       <c r="C32" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D32" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E32" t="n">
         <v>0</v>
@@ -997,10 +997,10 @@
         <v>7.75</v>
       </c>
       <c r="C33" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D33" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E33" t="n">
         <v>0</v>
@@ -1014,10 +1014,10 @@
         <v>8</v>
       </c>
       <c r="C34" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D34" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E34" t="n">
         <v>0</v>
@@ -1031,10 +1031,10 @@
         <v>8.25</v>
       </c>
       <c r="C35" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D35" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E35" t="n">
         <v>0</v>
@@ -1048,10 +1048,10 @@
         <v>8.5</v>
       </c>
       <c r="C36" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D36" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E36" t="n">
         <v>0</v>
@@ -1065,10 +1065,10 @@
         <v>8.75</v>
       </c>
       <c r="C37" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D37" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E37" t="n">
         <v>0</v>
@@ -1082,10 +1082,10 @@
         <v>9</v>
       </c>
       <c r="C38" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D38" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E38" t="n">
         <v>0</v>
@@ -1099,10 +1099,10 @@
         <v>9.25</v>
       </c>
       <c r="C39" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D39" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E39" t="n">
         <v>0</v>
@@ -1116,10 +1116,10 @@
         <v>9.5</v>
       </c>
       <c r="C40" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D40" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E40" t="n">
         <v>0</v>
@@ -1133,10 +1133,10 @@
         <v>9.75</v>
       </c>
       <c r="C41" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D41" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E41" t="n">
         <v>0</v>
@@ -1150,10 +1150,10 @@
         <v>10</v>
       </c>
       <c r="C42" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D42" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E42" t="n">
         <v>0</v>
@@ -1167,10 +1167,10 @@
         <v>10.25</v>
       </c>
       <c r="C43" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D43" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E43" t="n">
         <v>0</v>
@@ -1184,10 +1184,10 @@
         <v>10.5</v>
       </c>
       <c r="C44" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D44" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E44" t="n">
         <v>0</v>
@@ -1235,10 +1235,10 @@
         <v>11.25</v>
       </c>
       <c r="C47" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D47" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E47" t="n">
         <v>0</v>
@@ -1269,10 +1269,10 @@
         <v>11.75</v>
       </c>
       <c r="C49" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D49" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E49" t="n">
         <v>0</v>
@@ -1286,10 +1286,10 @@
         <v>12</v>
       </c>
       <c r="C50" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D50" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E50" t="n">
         <v>0</v>
@@ -1303,10 +1303,10 @@
         <v>12.25</v>
       </c>
       <c r="C51" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D51" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E51" t="n">
         <v>0</v>
@@ -1320,10 +1320,10 @@
         <v>12.5</v>
       </c>
       <c r="C52" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D52" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E52" t="n">
         <v>0</v>
@@ -1337,10 +1337,10 @@
         <v>12.75</v>
       </c>
       <c r="C53" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D53" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E53" t="n">
         <v>0</v>
@@ -1357,10 +1357,10 @@
         <v>5</v>
       </c>
       <c r="D54" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E54" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55">
@@ -1371,13 +1371,13 @@
         <v>13.25</v>
       </c>
       <c r="C55" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D55" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E55" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56">
@@ -1388,13 +1388,13 @@
         <v>13.5</v>
       </c>
       <c r="C56" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D56" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E56" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57">
@@ -1405,13 +1405,13 @@
         <v>13.75</v>
       </c>
       <c r="C57" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D57" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E57" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58">
@@ -1422,13 +1422,13 @@
         <v>14</v>
       </c>
       <c r="C58" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D58" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E58" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59">
@@ -1442,10 +1442,10 @@
         <v>1</v>
       </c>
       <c r="D59" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60">
@@ -1456,13 +1456,13 @@
         <v>14.5</v>
       </c>
       <c r="C60" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D60" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E60" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61">
@@ -1473,13 +1473,13 @@
         <v>14.75</v>
       </c>
       <c r="C61" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D61" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E61" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62">
@@ -1490,13 +1490,13 @@
         <v>15</v>
       </c>
       <c r="C62" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D62" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E62" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63">
@@ -1507,13 +1507,13 @@
         <v>15.25</v>
       </c>
       <c r="C63" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D63" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E63" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64">
@@ -1524,13 +1524,13 @@
         <v>15.5</v>
       </c>
       <c r="C64" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D64" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E64" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65">
@@ -1541,13 +1541,13 @@
         <v>15.75</v>
       </c>
       <c r="C65" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D65" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E65" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66">
@@ -1558,13 +1558,13 @@
         <v>16</v>
       </c>
       <c r="C66" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D66" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E66" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67">
@@ -1575,13 +1575,13 @@
         <v>16.25</v>
       </c>
       <c r="C67" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D67" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E67" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68">
@@ -1592,13 +1592,13 @@
         <v>16.5</v>
       </c>
       <c r="C68" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D68" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E68" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69">
@@ -1609,13 +1609,13 @@
         <v>16.75</v>
       </c>
       <c r="C69" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D69" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E69" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70">
@@ -1626,13 +1626,13 @@
         <v>17</v>
       </c>
       <c r="C70" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D70" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E70" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71">
@@ -1643,13 +1643,13 @@
         <v>17.25</v>
       </c>
       <c r="C71" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="D71" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E71" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72">
@@ -1660,13 +1660,13 @@
         <v>17.5</v>
       </c>
       <c r="C72" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D72" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E72" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73">
@@ -1677,13 +1677,13 @@
         <v>17.75</v>
       </c>
       <c r="C73" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D73" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E73" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74">
@@ -1694,13 +1694,13 @@
         <v>18</v>
       </c>
       <c r="C74" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D74" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E74" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75">
@@ -1711,13 +1711,13 @@
         <v>18.25</v>
       </c>
       <c r="C75" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D75" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E75" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76">
@@ -1728,13 +1728,13 @@
         <v>18.5</v>
       </c>
       <c r="C76" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D76" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E76" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77">
@@ -1745,13 +1745,13 @@
         <v>18.75</v>
       </c>
       <c r="C77" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D77" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E77" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78">
@@ -1762,13 +1762,13 @@
         <v>19</v>
       </c>
       <c r="C78" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D78" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E78" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79">
@@ -1779,13 +1779,13 @@
         <v>19.25</v>
       </c>
       <c r="C79" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D79" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E79" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="80">
@@ -1796,13 +1796,13 @@
         <v>19.5</v>
       </c>
       <c r="C80" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D80" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E80" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81">
@@ -1813,13 +1813,13 @@
         <v>19.75</v>
       </c>
       <c r="C81" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D81" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E81" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82">
@@ -1830,13 +1830,13 @@
         <v>20</v>
       </c>
       <c r="C82" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D82" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E82" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83">
@@ -1847,13 +1847,13 @@
         <v>20.25</v>
       </c>
       <c r="C83" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D83" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E83" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84">
@@ -1864,13 +1864,13 @@
         <v>20.5</v>
       </c>
       <c r="C84" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D84" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E84" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85">
@@ -1881,13 +1881,13 @@
         <v>20.75</v>
       </c>
       <c r="C85" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D85" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E85" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86">
@@ -1901,10 +1901,10 @@
         <v>10</v>
       </c>
       <c r="D86" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87">
@@ -1915,13 +1915,13 @@
         <v>21.25</v>
       </c>
       <c r="C87" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D87" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E87" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="88">
@@ -1935,10 +1935,10 @@
         <v>6</v>
       </c>
       <c r="D88" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E88" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89">
@@ -1949,13 +1949,13 @@
         <v>21.75</v>
       </c>
       <c r="C89" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D89" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E89" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="90">
@@ -1966,13 +1966,13 @@
         <v>22</v>
       </c>
       <c r="C90" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D90" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E90" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91">
@@ -1983,13 +1983,13 @@
         <v>22.25</v>
       </c>
       <c r="C91" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D91" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E91" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="92">
@@ -2000,13 +2000,13 @@
         <v>22.5</v>
       </c>
       <c r="C92" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D92" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E92" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="93">
@@ -2017,13 +2017,13 @@
         <v>22.75</v>
       </c>
       <c r="C93" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D93" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E93" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="94">
@@ -2034,13 +2034,13 @@
         <v>23</v>
       </c>
       <c r="C94" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D94" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E94" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="95">
@@ -2054,10 +2054,10 @@
         <v>8</v>
       </c>
       <c r="D95" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E95" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="96">
@@ -2068,13 +2068,13 @@
         <v>23.5</v>
       </c>
       <c r="C96" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D96" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E96" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="97">
@@ -2085,13 +2085,13 @@
         <v>23.75</v>
       </c>
       <c r="C97" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D97" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2710,7 +2710,7 @@
         <v>13</v>
       </c>
       <c r="C54" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55">
@@ -2721,7 +2721,7 @@
         <v>13.25</v>
       </c>
       <c r="C55" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56">
@@ -2732,7 +2732,7 @@
         <v>13.5</v>
       </c>
       <c r="C56" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57">
@@ -2743,7 +2743,7 @@
         <v>13.75</v>
       </c>
       <c r="C57" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58">
@@ -2754,7 +2754,7 @@
         <v>14</v>
       </c>
       <c r="C58" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59">
@@ -2765,7 +2765,7 @@
         <v>14.25</v>
       </c>
       <c r="C59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60">
@@ -2776,7 +2776,7 @@
         <v>14.5</v>
       </c>
       <c r="C60" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61">
@@ -2787,7 +2787,7 @@
         <v>14.75</v>
       </c>
       <c r="C61" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62">
@@ -2798,7 +2798,7 @@
         <v>15</v>
       </c>
       <c r="C62" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63">
@@ -2809,7 +2809,7 @@
         <v>15.25</v>
       </c>
       <c r="C63" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64">
@@ -2820,7 +2820,7 @@
         <v>15.5</v>
       </c>
       <c r="C64" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65">
@@ -2831,7 +2831,7 @@
         <v>15.75</v>
       </c>
       <c r="C65" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66">
@@ -2842,7 +2842,7 @@
         <v>16</v>
       </c>
       <c r="C66" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67">
@@ -2853,7 +2853,7 @@
         <v>16.25</v>
       </c>
       <c r="C67" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68">
@@ -2864,7 +2864,7 @@
         <v>16.5</v>
       </c>
       <c r="C68" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69">
@@ -2875,7 +2875,7 @@
         <v>16.75</v>
       </c>
       <c r="C69" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70">
@@ -2886,7 +2886,7 @@
         <v>17</v>
       </c>
       <c r="C70" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71">
@@ -2897,7 +2897,7 @@
         <v>17.25</v>
       </c>
       <c r="C71" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72">
@@ -2908,7 +2908,7 @@
         <v>17.5</v>
       </c>
       <c r="C72" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73">
@@ -2919,7 +2919,7 @@
         <v>17.75</v>
       </c>
       <c r="C73" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74">
@@ -2930,7 +2930,7 @@
         <v>18</v>
       </c>
       <c r="C74" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75">
@@ -2941,7 +2941,7 @@
         <v>18.25</v>
       </c>
       <c r="C75" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76">
@@ -2952,7 +2952,7 @@
         <v>18.5</v>
       </c>
       <c r="C76" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77">
@@ -2963,7 +2963,7 @@
         <v>18.75</v>
       </c>
       <c r="C77" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78">
@@ -2974,7 +2974,7 @@
         <v>19</v>
       </c>
       <c r="C78" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79">
@@ -2985,7 +2985,7 @@
         <v>19.25</v>
       </c>
       <c r="C79" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="80">
@@ -2996,7 +2996,7 @@
         <v>19.5</v>
       </c>
       <c r="C80" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81">
@@ -3007,7 +3007,7 @@
         <v>19.75</v>
       </c>
       <c r="C81" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82">
@@ -3018,7 +3018,7 @@
         <v>20</v>
       </c>
       <c r="C82" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83">
@@ -3029,7 +3029,7 @@
         <v>20.25</v>
       </c>
       <c r="C83" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84">
@@ -3040,7 +3040,7 @@
         <v>20.5</v>
       </c>
       <c r="C84" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85">
@@ -3051,7 +3051,7 @@
         <v>20.75</v>
       </c>
       <c r="C85" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86">
@@ -3062,7 +3062,7 @@
         <v>21</v>
       </c>
       <c r="C86" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87">
@@ -3073,7 +3073,7 @@
         <v>21.25</v>
       </c>
       <c r="C87" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="88">
@@ -3084,7 +3084,7 @@
         <v>21.5</v>
       </c>
       <c r="C88" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89">
@@ -3095,7 +3095,7 @@
         <v>21.75</v>
       </c>
       <c r="C89" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="90">
@@ -3106,7 +3106,7 @@
         <v>22</v>
       </c>
       <c r="C90" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91">
@@ -3117,7 +3117,7 @@
         <v>22.25</v>
       </c>
       <c r="C91" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="92">
@@ -3128,7 +3128,7 @@
         <v>22.5</v>
       </c>
       <c r="C92" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="93">
@@ -3139,7 +3139,7 @@
         <v>22.75</v>
       </c>
       <c r="C93" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="94">
@@ -3150,7 +3150,7 @@
         <v>23</v>
       </c>
       <c r="C94" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="95">
@@ -3161,7 +3161,7 @@
         <v>23.25</v>
       </c>
       <c r="C95" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="96">
@@ -3172,7 +3172,7 @@
         <v>23.5</v>
       </c>
       <c r="C96" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="97">
@@ -3183,7 +3183,7 @@
         <v>23.75</v>
       </c>
       <c r="C97" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3240,13 +3240,13 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D2" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E2" t="n">
-        <v>1</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="3">
@@ -3257,13 +3257,13 @@
         <v>0.25</v>
       </c>
       <c r="C3" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="4">
@@ -3274,13 +3274,13 @@
         <v>0.5</v>
       </c>
       <c r="C4" t="n">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="D4" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="5">
@@ -3291,13 +3291,13 @@
         <v>0.75</v>
       </c>
       <c r="C5" t="n">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="D5" t="n">
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>1</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="6">
@@ -3308,13 +3308,13 @@
         <v>1</v>
       </c>
       <c r="C6" t="n">
-        <v>9</v>
+        <v>54</v>
       </c>
       <c r="D6" t="n">
         <v>9</v>
       </c>
       <c r="E6" t="n">
-        <v>1</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="7">
@@ -3325,13 +3325,13 @@
         <v>1.25</v>
       </c>
       <c r="C7" t="n">
-        <v>1</v>
+        <v>54</v>
       </c>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E7" t="n">
-        <v>1</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="8">
@@ -3342,13 +3342,13 @@
         <v>1.5</v>
       </c>
       <c r="C8" t="n">
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="D8" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E8" t="n">
-        <v>1</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="9">
@@ -3359,13 +3359,13 @@
         <v>1.75</v>
       </c>
       <c r="C9" t="n">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="D9" t="n">
         <v>3</v>
       </c>
       <c r="E9" t="n">
-        <v>1</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="10">
@@ -3376,13 +3376,13 @@
         <v>2</v>
       </c>
       <c r="C10" t="n">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="D10" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E10" t="n">
-        <v>1</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="11">
@@ -3393,13 +3393,13 @@
         <v>2.25</v>
       </c>
       <c r="C11" t="n">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="D11" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E11" t="n">
-        <v>1</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="12">
@@ -3410,13 +3410,13 @@
         <v>2.5</v>
       </c>
       <c r="C12" t="n">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="D12" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E12" t="n">
-        <v>1</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="13">
@@ -3427,13 +3427,13 @@
         <v>2.75</v>
       </c>
       <c r="C13" t="n">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="D13" t="n">
         <v>8</v>
       </c>
       <c r="E13" t="n">
-        <v>1</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="14">
@@ -3444,13 +3444,13 @@
         <v>3</v>
       </c>
       <c r="C14" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D14" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E14" t="n">
-        <v>1</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="15">
@@ -3461,13 +3461,13 @@
         <v>3.25</v>
       </c>
       <c r="C15" t="n">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="D15" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E15" t="n">
-        <v>1</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="16">
@@ -3478,13 +3478,13 @@
         <v>3.5</v>
       </c>
       <c r="C16" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D16" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E16" t="n">
-        <v>1</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="17">
@@ -3495,13 +3495,13 @@
         <v>3.75</v>
       </c>
       <c r="C17" t="n">
-        <v>10</v>
+        <v>48</v>
       </c>
       <c r="D17" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E17" t="n">
-        <v>1</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="18">
@@ -3512,13 +3512,13 @@
         <v>4</v>
       </c>
       <c r="C18" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D18" t="n">
         <v>2</v>
       </c>
       <c r="E18" t="n">
-        <v>1</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="19">
@@ -3529,13 +3529,13 @@
         <v>4.25</v>
       </c>
       <c r="C19" t="n">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="D19" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E19" t="n">
-        <v>1</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="20">
@@ -3546,13 +3546,13 @@
         <v>4.5</v>
       </c>
       <c r="C20" t="n">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="D20" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E20" t="n">
-        <v>1</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="21">
@@ -3563,13 +3563,13 @@
         <v>4.75</v>
       </c>
       <c r="C21" t="n">
-        <v>6</v>
+        <v>54</v>
       </c>
       <c r="D21" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E21" t="n">
-        <v>1</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="22">
@@ -3580,13 +3580,13 @@
         <v>5</v>
       </c>
       <c r="C22" t="n">
-        <v>2</v>
+        <v>54</v>
       </c>
       <c r="D22" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="E22" t="n">
-        <v>1</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="23">
@@ -3597,13 +3597,13 @@
         <v>5.25</v>
       </c>
       <c r="C23" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D23" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E23" t="n">
-        <v>1</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="24">
@@ -3614,13 +3614,13 @@
         <v>5.5</v>
       </c>
       <c r="C24" t="n">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="D24" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E24" t="n">
-        <v>1</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="25">
@@ -3631,13 +3631,13 @@
         <v>5.75</v>
       </c>
       <c r="C25" t="n">
-        <v>4</v>
+        <v>36</v>
       </c>
       <c r="D25" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E25" t="n">
-        <v>1</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="26">
@@ -3648,13 +3648,13 @@
         <v>6</v>
       </c>
       <c r="C26" t="n">
-        <v>3</v>
+        <v>48</v>
       </c>
       <c r="D26" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E26" t="n">
-        <v>1</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="27">
@@ -3668,10 +3668,10 @@
         <v>6</v>
       </c>
       <c r="D27" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E27" t="n">
-        <v>1</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="28">
@@ -3682,13 +3682,13 @@
         <v>6.5</v>
       </c>
       <c r="C28" t="n">
-        <v>2</v>
+        <v>42</v>
       </c>
       <c r="D28" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E28" t="n">
-        <v>1</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="29">
@@ -3699,13 +3699,13 @@
         <v>6.75</v>
       </c>
       <c r="C29" t="n">
-        <v>3</v>
+        <v>60</v>
       </c>
       <c r="D29" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>1</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="30">
@@ -3716,13 +3716,13 @@
         <v>7</v>
       </c>
       <c r="C30" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D30" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E30" t="n">
-        <v>1</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="31">
@@ -3733,13 +3733,13 @@
         <v>7.25</v>
       </c>
       <c r="C31" t="n">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="D31" t="n">
         <v>3</v>
       </c>
       <c r="E31" t="n">
-        <v>1</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="32">
@@ -3750,13 +3750,13 @@
         <v>7.5</v>
       </c>
       <c r="C32" t="n">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="D32" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E32" t="n">
-        <v>1</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="33">
@@ -3767,13 +3767,13 @@
         <v>7.75</v>
       </c>
       <c r="C33" t="n">
-        <v>6</v>
+        <v>54</v>
       </c>
       <c r="D33" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E33" t="n">
-        <v>1</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="34">
@@ -3784,13 +3784,13 @@
         <v>8</v>
       </c>
       <c r="C34" t="n">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="D34" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E34" t="n">
-        <v>1</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="35">
@@ -3801,13 +3801,13 @@
         <v>8.25</v>
       </c>
       <c r="C35" t="n">
-        <v>8</v>
+        <v>54</v>
       </c>
       <c r="D35" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E35" t="n">
-        <v>1</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="36">
@@ -3818,13 +3818,13 @@
         <v>8.5</v>
       </c>
       <c r="C36" t="n">
-        <v>10</v>
+        <v>54</v>
       </c>
       <c r="D36" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E36" t="n">
-        <v>1</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="37">
@@ -3835,13 +3835,13 @@
         <v>8.75</v>
       </c>
       <c r="C37" t="n">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="D37" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E37" t="n">
-        <v>1</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="38">
@@ -3852,13 +3852,13 @@
         <v>9</v>
       </c>
       <c r="C38" t="n">
-        <v>3</v>
+        <v>54</v>
       </c>
       <c r="D38" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E38" t="n">
-        <v>1</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="39">
@@ -3869,13 +3869,13 @@
         <v>9.25</v>
       </c>
       <c r="C39" t="n">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="D39" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E39" t="n">
-        <v>1</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="40">
@@ -3886,13 +3886,13 @@
         <v>9.5</v>
       </c>
       <c r="C40" t="n">
-        <v>3</v>
+        <v>54</v>
       </c>
       <c r="D40" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E40" t="n">
-        <v>1</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="41">
@@ -3903,13 +3903,13 @@
         <v>9.75</v>
       </c>
       <c r="C41" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D41" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E41" t="n">
-        <v>1</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="42">
@@ -3920,13 +3920,13 @@
         <v>10</v>
       </c>
       <c r="C42" t="n">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="D42" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>1</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="43">
@@ -3937,13 +3937,13 @@
         <v>10.25</v>
       </c>
       <c r="C43" t="n">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="D43" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E43" t="n">
-        <v>1</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="44">
@@ -3954,13 +3954,13 @@
         <v>10.5</v>
       </c>
       <c r="C44" t="n">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="D44" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E44" t="n">
-        <v>1</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="45">
@@ -3971,13 +3971,13 @@
         <v>10.75</v>
       </c>
       <c r="C45" t="n">
-        <v>9</v>
+        <v>54</v>
       </c>
       <c r="D45" t="n">
         <v>9</v>
       </c>
       <c r="E45" t="n">
-        <v>1</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="46">
@@ -3988,13 +3988,13 @@
         <v>11</v>
       </c>
       <c r="C46" t="n">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="D46" t="n">
         <v>8</v>
       </c>
       <c r="E46" t="n">
-        <v>1</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="47">
@@ -4005,13 +4005,13 @@
         <v>11.25</v>
       </c>
       <c r="C47" t="n">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D47" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E47" t="n">
-        <v>1</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="48">
@@ -4022,13 +4022,13 @@
         <v>11.5</v>
       </c>
       <c r="C48" t="n">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D48" t="n">
         <v>6</v>
       </c>
       <c r="E48" t="n">
-        <v>1</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="49">
@@ -4039,13 +4039,13 @@
         <v>11.75</v>
       </c>
       <c r="C49" t="n">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="D49" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E49" t="n">
-        <v>1</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="50">
@@ -4056,13 +4056,13 @@
         <v>12</v>
       </c>
       <c r="C50" t="n">
-        <v>6</v>
+        <v>54</v>
       </c>
       <c r="D50" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E50" t="n">
-        <v>1</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="51">
@@ -4073,13 +4073,13 @@
         <v>12.25</v>
       </c>
       <c r="C51" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D51" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E51" t="n">
-        <v>1</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="52">
@@ -4090,13 +4090,13 @@
         <v>12.5</v>
       </c>
       <c r="C52" t="n">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="D52" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E52" t="n">
-        <v>1</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="53">
@@ -4107,13 +4107,13 @@
         <v>12.75</v>
       </c>
       <c r="C53" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D53" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E53" t="n">
-        <v>1</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="54">
@@ -4124,13 +4124,13 @@
         <v>13</v>
       </c>
       <c r="C54" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="D54" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E54" t="n">
-        <v>0</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="55">
@@ -4141,13 +4141,13 @@
         <v>13.25</v>
       </c>
       <c r="C55" t="n">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="D55" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E55" t="n">
-        <v>0</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="56">
@@ -4158,13 +4158,13 @@
         <v>13.5</v>
       </c>
       <c r="C56" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="D56" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E56" t="n">
-        <v>0</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="57">
@@ -4175,13 +4175,13 @@
         <v>13.75</v>
       </c>
       <c r="C57" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D57" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E57" t="n">
-        <v>0</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="58">
@@ -4192,13 +4192,13 @@
         <v>14</v>
       </c>
       <c r="C58" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D58" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E58" t="n">
-        <v>0</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="59">
@@ -4209,13 +4209,13 @@
         <v>14.25</v>
       </c>
       <c r="C59" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D59" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E59" t="n">
-        <v>0</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="60">
@@ -4226,13 +4226,13 @@
         <v>14.5</v>
       </c>
       <c r="C60" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="D60" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E60" t="n">
-        <v>0</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="61">
@@ -4243,13 +4243,13 @@
         <v>14.75</v>
       </c>
       <c r="C61" t="n">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="D61" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E61" t="n">
-        <v>0</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="62">
@@ -4260,13 +4260,13 @@
         <v>15</v>
       </c>
       <c r="C62" t="n">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="D62" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E62" t="n">
-        <v>0</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="63">
@@ -4277,13 +4277,13 @@
         <v>15.25</v>
       </c>
       <c r="C63" t="n">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="D63" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E63" t="n">
-        <v>0</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="64">
@@ -4294,13 +4294,13 @@
         <v>15.5</v>
       </c>
       <c r="C64" t="n">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="D64" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E64" t="n">
-        <v>0</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="65">
@@ -4311,13 +4311,13 @@
         <v>15.75</v>
       </c>
       <c r="C65" t="n">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="D65" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E65" t="n">
-        <v>0</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="66">
@@ -4328,13 +4328,13 @@
         <v>16</v>
       </c>
       <c r="C66" t="n">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="D66" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E66" t="n">
-        <v>0</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="67">
@@ -4345,13 +4345,13 @@
         <v>16.25</v>
       </c>
       <c r="C67" t="n">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="D67" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E67" t="n">
-        <v>0</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="68">
@@ -4362,13 +4362,13 @@
         <v>16.5</v>
       </c>
       <c r="C68" t="n">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="D68" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E68" t="n">
-        <v>0</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="69">
@@ -4379,13 +4379,13 @@
         <v>16.75</v>
       </c>
       <c r="C69" t="n">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="D69" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E69" t="n">
-        <v>0</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="70">
@@ -4396,13 +4396,13 @@
         <v>17</v>
       </c>
       <c r="C70" t="n">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="D70" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E70" t="n">
-        <v>0</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="71">
@@ -4413,13 +4413,13 @@
         <v>17.25</v>
       </c>
       <c r="C71" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="D71" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E71" t="n">
-        <v>0</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="72">
@@ -4430,13 +4430,13 @@
         <v>17.5</v>
       </c>
       <c r="C72" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="D72" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E72" t="n">
-        <v>0</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="73">
@@ -4447,13 +4447,13 @@
         <v>17.75</v>
       </c>
       <c r="C73" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D73" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E73" t="n">
-        <v>0</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="74">
@@ -4464,13 +4464,13 @@
         <v>18</v>
       </c>
       <c r="C74" t="n">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="D74" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E74" t="n">
-        <v>0</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="75">
@@ -4481,13 +4481,13 @@
         <v>18.25</v>
       </c>
       <c r="C75" t="n">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="D75" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E75" t="n">
-        <v>0</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="76">
@@ -4498,13 +4498,13 @@
         <v>18.5</v>
       </c>
       <c r="C76" t="n">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="D76" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E76" t="n">
-        <v>0</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="77">
@@ -4515,13 +4515,13 @@
         <v>18.75</v>
       </c>
       <c r="C77" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D77" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E77" t="n">
-        <v>0</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="78">
@@ -4532,13 +4532,13 @@
         <v>19</v>
       </c>
       <c r="C78" t="n">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="D78" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E78" t="n">
-        <v>0</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="79">
@@ -4549,13 +4549,13 @@
         <v>19.25</v>
       </c>
       <c r="C79" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D79" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E79" t="n">
-        <v>0</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="80">
@@ -4566,13 +4566,13 @@
         <v>19.5</v>
       </c>
       <c r="C80" t="n">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="D80" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E80" t="n">
-        <v>0</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="81">
@@ -4583,13 +4583,13 @@
         <v>19.75</v>
       </c>
       <c r="C81" t="n">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="D81" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E81" t="n">
-        <v>0</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="82">
@@ -4600,13 +4600,13 @@
         <v>20</v>
       </c>
       <c r="C82" t="n">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="D82" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E82" t="n">
-        <v>0</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="83">
@@ -4617,13 +4617,13 @@
         <v>20.25</v>
       </c>
       <c r="C83" t="n">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="D83" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E83" t="n">
-        <v>0</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="84">
@@ -4634,13 +4634,13 @@
         <v>20.5</v>
       </c>
       <c r="C84" t="n">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="D84" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E84" t="n">
-        <v>0</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="85">
@@ -4651,13 +4651,13 @@
         <v>20.75</v>
       </c>
       <c r="C85" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D85" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E85" t="n">
-        <v>0</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="86">
@@ -4668,13 +4668,13 @@
         <v>21</v>
       </c>
       <c r="C86" t="n">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="D86" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>0</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="87">
@@ -4685,13 +4685,13 @@
         <v>21.25</v>
       </c>
       <c r="C87" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D87" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E87" t="n">
-        <v>0</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="88">
@@ -4702,13 +4702,13 @@
         <v>21.5</v>
       </c>
       <c r="C88" t="n">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="D88" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E88" t="n">
-        <v>0</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="89">
@@ -4719,13 +4719,13 @@
         <v>21.75</v>
       </c>
       <c r="C89" t="n">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="D89" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E89" t="n">
-        <v>0</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="90">
@@ -4736,13 +4736,13 @@
         <v>22</v>
       </c>
       <c r="C90" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="D90" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E90" t="n">
-        <v>0</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="91">
@@ -4753,13 +4753,13 @@
         <v>22.25</v>
       </c>
       <c r="C91" t="n">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="D91" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E91" t="n">
-        <v>0</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="92">
@@ -4770,13 +4770,13 @@
         <v>22.5</v>
       </c>
       <c r="C92" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D92" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E92" t="n">
-        <v>0</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="93">
@@ -4787,13 +4787,13 @@
         <v>22.75</v>
       </c>
       <c r="C93" t="n">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="D93" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E93" t="n">
-        <v>0</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="94">
@@ -4804,13 +4804,13 @@
         <v>23</v>
       </c>
       <c r="C94" t="n">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="D94" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E94" t="n">
-        <v>0</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="95">
@@ -4821,13 +4821,13 @@
         <v>23.25</v>
       </c>
       <c r="C95" t="n">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="D95" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E95" t="n">
-        <v>0</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="96">
@@ -4838,13 +4838,13 @@
         <v>23.5</v>
       </c>
       <c r="C96" t="n">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="D96" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E96" t="n">
-        <v>0</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="97">
@@ -4855,13 +4855,13 @@
         <v>23.75</v>
       </c>
       <c r="C97" t="n">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="D97" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>0</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Add simulation application and core solver engine, updating timeseries results spreadsheet.
</commit_message>
<xml_diff>
--- a/timeseries_results.xlsx
+++ b/timeseries_results.xlsx
@@ -2088,10 +2088,10 @@
         <v>10</v>
       </c>
       <c r="D97" t="n">
+        <v>0</v>
+      </c>
+      <c r="E97" t="n">
         <v>10</v>
-      </c>
-      <c r="E97" t="n">
-        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3183,7 +3183,7 @@
         <v>23.75</v>
       </c>
       <c r="C97" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -3240,13 +3240,13 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D2" t="n">
         <v>2</v>
       </c>
       <c r="E2" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.3333333333333333</v>
       </c>
     </row>
     <row r="3">
@@ -3274,13 +3274,13 @@
         <v>0.5</v>
       </c>
       <c r="C4" t="n">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="D4" t="n">
         <v>6</v>
       </c>
       <c r="E4" t="n">
-        <v>0.1666666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -3291,13 +3291,13 @@
         <v>0.75</v>
       </c>
       <c r="C5" t="n">
-        <v>60</v>
+        <v>12</v>
       </c>
       <c r="D5" t="n">
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.8333333333333334</v>
       </c>
     </row>
     <row r="6">
@@ -3308,13 +3308,13 @@
         <v>1</v>
       </c>
       <c r="C6" t="n">
-        <v>54</v>
+        <v>12</v>
       </c>
       <c r="D6" t="n">
         <v>9</v>
       </c>
       <c r="E6" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="7">
@@ -3325,13 +3325,13 @@
         <v>1.25</v>
       </c>
       <c r="C7" t="n">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="D7" t="n">
         <v>9</v>
       </c>
       <c r="E7" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="8">
@@ -3342,13 +3342,13 @@
         <v>1.5</v>
       </c>
       <c r="C8" t="n">
-        <v>48</v>
+        <v>12</v>
       </c>
       <c r="D8" t="n">
         <v>8</v>
       </c>
       <c r="E8" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.6666666666666666</v>
       </c>
     </row>
     <row r="9">
@@ -3359,13 +3359,13 @@
         <v>1.75</v>
       </c>
       <c r="C9" t="n">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="D9" t="n">
         <v>3</v>
       </c>
       <c r="E9" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="10">
@@ -3376,13 +3376,13 @@
         <v>2</v>
       </c>
       <c r="C10" t="n">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="D10" t="n">
         <v>4</v>
       </c>
       <c r="E10" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.6666666666666666</v>
       </c>
     </row>
     <row r="11">
@@ -3393,13 +3393,13 @@
         <v>2.25</v>
       </c>
       <c r="C11" t="n">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="D11" t="n">
         <v>6</v>
       </c>
       <c r="E11" t="n">
-        <v>0.1666666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
@@ -3410,13 +3410,13 @@
         <v>2.5</v>
       </c>
       <c r="C12" t="n">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="D12" t="n">
         <v>3</v>
       </c>
       <c r="E12" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="13">
@@ -3427,13 +3427,13 @@
         <v>2.75</v>
       </c>
       <c r="C13" t="n">
-        <v>48</v>
+        <v>12</v>
       </c>
       <c r="D13" t="n">
         <v>8</v>
       </c>
       <c r="E13" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.6666666666666666</v>
       </c>
     </row>
     <row r="14">
@@ -3461,13 +3461,13 @@
         <v>3.25</v>
       </c>
       <c r="C15" t="n">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="D15" t="n">
         <v>7</v>
       </c>
       <c r="E15" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.5833333333333334</v>
       </c>
     </row>
     <row r="16">
@@ -3478,13 +3478,13 @@
         <v>3.5</v>
       </c>
       <c r="C16" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D16" t="n">
         <v>2</v>
       </c>
       <c r="E16" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.3333333333333333</v>
       </c>
     </row>
     <row r="17">
@@ -3495,13 +3495,13 @@
         <v>3.75</v>
       </c>
       <c r="C17" t="n">
-        <v>48</v>
+        <v>12</v>
       </c>
       <c r="D17" t="n">
         <v>8</v>
       </c>
       <c r="E17" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.6666666666666666</v>
       </c>
     </row>
     <row r="18">
@@ -3512,13 +3512,13 @@
         <v>4</v>
       </c>
       <c r="C18" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D18" t="n">
         <v>2</v>
       </c>
       <c r="E18" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.3333333333333333</v>
       </c>
     </row>
     <row r="19">
@@ -3529,13 +3529,13 @@
         <v>4.25</v>
       </c>
       <c r="C19" t="n">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="D19" t="n">
         <v>5</v>
       </c>
       <c r="E19" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.8333333333333334</v>
       </c>
     </row>
     <row r="20">
@@ -3546,13 +3546,13 @@
         <v>4.5</v>
       </c>
       <c r="C20" t="n">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="D20" t="n">
         <v>7</v>
       </c>
       <c r="E20" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.5833333333333334</v>
       </c>
     </row>
     <row r="21">
@@ -3563,13 +3563,13 @@
         <v>4.75</v>
       </c>
       <c r="C21" t="n">
-        <v>54</v>
+        <v>12</v>
       </c>
       <c r="D21" t="n">
         <v>9</v>
       </c>
       <c r="E21" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="22">
@@ -3580,13 +3580,13 @@
         <v>5</v>
       </c>
       <c r="C22" t="n">
-        <v>54</v>
+        <v>12</v>
       </c>
       <c r="D22" t="n">
         <v>9</v>
       </c>
       <c r="E22" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="23">
@@ -3614,13 +3614,13 @@
         <v>5.5</v>
       </c>
       <c r="C24" t="n">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="D24" t="n">
         <v>4</v>
       </c>
       <c r="E24" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.6666666666666666</v>
       </c>
     </row>
     <row r="25">
@@ -3631,13 +3631,13 @@
         <v>5.75</v>
       </c>
       <c r="C25" t="n">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="D25" t="n">
         <v>6</v>
       </c>
       <c r="E25" t="n">
-        <v>0.1666666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26">
@@ -3648,13 +3648,13 @@
         <v>6</v>
       </c>
       <c r="C26" t="n">
-        <v>48</v>
+        <v>12</v>
       </c>
       <c r="D26" t="n">
         <v>8</v>
       </c>
       <c r="E26" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.6666666666666666</v>
       </c>
     </row>
     <row r="27">
@@ -3682,13 +3682,13 @@
         <v>6.5</v>
       </c>
       <c r="C28" t="n">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="D28" t="n">
         <v>7</v>
       </c>
       <c r="E28" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.5833333333333334</v>
       </c>
     </row>
     <row r="29">
@@ -3699,13 +3699,13 @@
         <v>6.75</v>
       </c>
       <c r="C29" t="n">
-        <v>60</v>
+        <v>12</v>
       </c>
       <c r="D29" t="n">
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.8333333333333334</v>
       </c>
     </row>
     <row r="30">
@@ -3733,13 +3733,13 @@
         <v>7.25</v>
       </c>
       <c r="C31" t="n">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="D31" t="n">
         <v>3</v>
       </c>
       <c r="E31" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="32">
@@ -3750,13 +3750,13 @@
         <v>7.5</v>
       </c>
       <c r="C32" t="n">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="D32" t="n">
         <v>6</v>
       </c>
       <c r="E32" t="n">
-        <v>0.1666666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33">
@@ -3767,13 +3767,13 @@
         <v>7.75</v>
       </c>
       <c r="C33" t="n">
-        <v>54</v>
+        <v>12</v>
       </c>
       <c r="D33" t="n">
         <v>9</v>
       </c>
       <c r="E33" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="34">
@@ -3784,13 +3784,13 @@
         <v>8</v>
       </c>
       <c r="C34" t="n">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="D34" t="n">
         <v>7</v>
       </c>
       <c r="E34" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.5833333333333334</v>
       </c>
     </row>
     <row r="35">
@@ -3801,13 +3801,13 @@
         <v>8.25</v>
       </c>
       <c r="C35" t="n">
-        <v>54</v>
+        <v>12</v>
       </c>
       <c r="D35" t="n">
         <v>9</v>
       </c>
       <c r="E35" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="36">
@@ -3818,13 +3818,13 @@
         <v>8.5</v>
       </c>
       <c r="C36" t="n">
-        <v>54</v>
+        <v>12</v>
       </c>
       <c r="D36" t="n">
         <v>9</v>
       </c>
       <c r="E36" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="37">
@@ -3835,13 +3835,13 @@
         <v>8.75</v>
       </c>
       <c r="C37" t="n">
-        <v>48</v>
+        <v>12</v>
       </c>
       <c r="D37" t="n">
         <v>8</v>
       </c>
       <c r="E37" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.6666666666666666</v>
       </c>
     </row>
     <row r="38">
@@ -3852,13 +3852,13 @@
         <v>9</v>
       </c>
       <c r="C38" t="n">
-        <v>54</v>
+        <v>12</v>
       </c>
       <c r="D38" t="n">
         <v>9</v>
       </c>
       <c r="E38" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="39">
@@ -3869,13 +3869,13 @@
         <v>9.25</v>
       </c>
       <c r="C39" t="n">
-        <v>48</v>
+        <v>12</v>
       </c>
       <c r="D39" t="n">
         <v>8</v>
       </c>
       <c r="E39" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.6666666666666666</v>
       </c>
     </row>
     <row r="40">
@@ -3886,13 +3886,13 @@
         <v>9.5</v>
       </c>
       <c r="C40" t="n">
-        <v>54</v>
+        <v>12</v>
       </c>
       <c r="D40" t="n">
         <v>9</v>
       </c>
       <c r="E40" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="41">
@@ -3920,13 +3920,13 @@
         <v>10</v>
       </c>
       <c r="C42" t="n">
-        <v>60</v>
+        <v>12</v>
       </c>
       <c r="D42" t="n">
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.8333333333333334</v>
       </c>
     </row>
     <row r="43">
@@ -3937,13 +3937,13 @@
         <v>10.25</v>
       </c>
       <c r="C43" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D43" t="n">
         <v>2</v>
       </c>
       <c r="E43" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.3333333333333333</v>
       </c>
     </row>
     <row r="44">
@@ -3954,13 +3954,13 @@
         <v>10.5</v>
       </c>
       <c r="C44" t="n">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="D44" t="n">
         <v>6</v>
       </c>
       <c r="E44" t="n">
-        <v>0.1666666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45">
@@ -3971,13 +3971,13 @@
         <v>10.75</v>
       </c>
       <c r="C45" t="n">
-        <v>54</v>
+        <v>12</v>
       </c>
       <c r="D45" t="n">
         <v>9</v>
       </c>
       <c r="E45" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="46">
@@ -3988,13 +3988,13 @@
         <v>11</v>
       </c>
       <c r="C46" t="n">
-        <v>48</v>
+        <v>12</v>
       </c>
       <c r="D46" t="n">
         <v>8</v>
       </c>
       <c r="E46" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.6666666666666666</v>
       </c>
     </row>
     <row r="47">
@@ -4005,13 +4005,13 @@
         <v>11.25</v>
       </c>
       <c r="C47" t="n">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="D47" t="n">
         <v>3</v>
       </c>
       <c r="E47" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="48">
@@ -4022,13 +4022,13 @@
         <v>11.5</v>
       </c>
       <c r="C48" t="n">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="D48" t="n">
         <v>6</v>
       </c>
       <c r="E48" t="n">
-        <v>0.1666666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49">
@@ -4039,13 +4039,13 @@
         <v>11.75</v>
       </c>
       <c r="C49" t="n">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="D49" t="n">
         <v>5</v>
       </c>
       <c r="E49" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.8333333333333334</v>
       </c>
     </row>
     <row r="50">
@@ -4056,13 +4056,13 @@
         <v>12</v>
       </c>
       <c r="C50" t="n">
-        <v>54</v>
+        <v>12</v>
       </c>
       <c r="D50" t="n">
         <v>9</v>
       </c>
       <c r="E50" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="51">
@@ -4090,13 +4090,13 @@
         <v>12.5</v>
       </c>
       <c r="C52" t="n">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="D52" t="n">
         <v>5</v>
       </c>
       <c r="E52" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.8333333333333334</v>
       </c>
     </row>
     <row r="53">
@@ -4124,13 +4124,13 @@
         <v>13</v>
       </c>
       <c r="C54" t="n">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="D54" t="n">
         <v>5</v>
       </c>
       <c r="E54" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.8333333333333334</v>
       </c>
     </row>
     <row r="55">
@@ -4141,13 +4141,13 @@
         <v>13.25</v>
       </c>
       <c r="C55" t="n">
-        <v>48</v>
+        <v>12</v>
       </c>
       <c r="D55" t="n">
         <v>8</v>
       </c>
       <c r="E55" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.6666666666666666</v>
       </c>
     </row>
     <row r="56">
@@ -4158,13 +4158,13 @@
         <v>13.5</v>
       </c>
       <c r="C56" t="n">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="D56" t="n">
         <v>5</v>
       </c>
       <c r="E56" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.8333333333333334</v>
       </c>
     </row>
     <row r="57">
@@ -4175,13 +4175,13 @@
         <v>13.75</v>
       </c>
       <c r="C57" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D57" t="n">
         <v>2</v>
       </c>
       <c r="E57" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.3333333333333333</v>
       </c>
     </row>
     <row r="58">
@@ -4192,13 +4192,13 @@
         <v>14</v>
       </c>
       <c r="C58" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D58" t="n">
         <v>2</v>
       </c>
       <c r="E58" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.3333333333333333</v>
       </c>
     </row>
     <row r="59">
@@ -4226,13 +4226,13 @@
         <v>14.5</v>
       </c>
       <c r="C60" t="n">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="D60" t="n">
         <v>3</v>
       </c>
       <c r="E60" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="61">
@@ -4243,13 +4243,13 @@
         <v>14.75</v>
       </c>
       <c r="C61" t="n">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="D61" t="n">
         <v>6</v>
       </c>
       <c r="E61" t="n">
-        <v>0.1666666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62">
@@ -4260,13 +4260,13 @@
         <v>15</v>
       </c>
       <c r="C62" t="n">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="D62" t="n">
         <v>6</v>
       </c>
       <c r="E62" t="n">
-        <v>0.1666666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63">
@@ -4277,13 +4277,13 @@
         <v>15.25</v>
       </c>
       <c r="C63" t="n">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="D63" t="n">
         <v>4</v>
       </c>
       <c r="E63" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.6666666666666666</v>
       </c>
     </row>
     <row r="64">
@@ -4294,13 +4294,13 @@
         <v>15.5</v>
       </c>
       <c r="C64" t="n">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="D64" t="n">
         <v>4</v>
       </c>
       <c r="E64" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.6666666666666666</v>
       </c>
     </row>
     <row r="65">
@@ -4311,13 +4311,13 @@
         <v>15.75</v>
       </c>
       <c r="C65" t="n">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="D65" t="n">
         <v>7</v>
       </c>
       <c r="E65" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.5833333333333334</v>
       </c>
     </row>
     <row r="66">
@@ -4328,13 +4328,13 @@
         <v>16</v>
       </c>
       <c r="C66" t="n">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="D66" t="n">
         <v>6</v>
       </c>
       <c r="E66" t="n">
-        <v>0.1666666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67">
@@ -4345,13 +4345,13 @@
         <v>16.25</v>
       </c>
       <c r="C67" t="n">
-        <v>54</v>
+        <v>12</v>
       </c>
       <c r="D67" t="n">
         <v>9</v>
       </c>
       <c r="E67" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="68">
@@ -4362,13 +4362,13 @@
         <v>16.5</v>
       </c>
       <c r="C68" t="n">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="D68" t="n">
         <v>7</v>
       </c>
       <c r="E68" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.5833333333333334</v>
       </c>
     </row>
     <row r="69">
@@ -4379,13 +4379,13 @@
         <v>16.75</v>
       </c>
       <c r="C69" t="n">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="D69" t="n">
         <v>6</v>
       </c>
       <c r="E69" t="n">
-        <v>0.1666666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70">
@@ -4396,13 +4396,13 @@
         <v>17</v>
       </c>
       <c r="C70" t="n">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="D70" t="n">
         <v>4</v>
       </c>
       <c r="E70" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.6666666666666666</v>
       </c>
     </row>
     <row r="71">
@@ -4413,13 +4413,13 @@
         <v>17.25</v>
       </c>
       <c r="C71" t="n">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="D71" t="n">
         <v>3</v>
       </c>
       <c r="E71" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="72">
@@ -4430,13 +4430,13 @@
         <v>17.5</v>
       </c>
       <c r="C72" t="n">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="D72" t="n">
         <v>3</v>
       </c>
       <c r="E72" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="73">
@@ -4447,13 +4447,13 @@
         <v>17.75</v>
       </c>
       <c r="C73" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D73" t="n">
         <v>2</v>
       </c>
       <c r="E73" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.3333333333333333</v>
       </c>
     </row>
     <row r="74">
@@ -4464,13 +4464,13 @@
         <v>18</v>
       </c>
       <c r="C74" t="n">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="D74" t="n">
         <v>4</v>
       </c>
       <c r="E74" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.6666666666666666</v>
       </c>
     </row>
     <row r="75">
@@ -4481,13 +4481,13 @@
         <v>18.25</v>
       </c>
       <c r="C75" t="n">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="D75" t="n">
         <v>7</v>
       </c>
       <c r="E75" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.5833333333333334</v>
       </c>
     </row>
     <row r="76">
@@ -4498,13 +4498,13 @@
         <v>18.5</v>
       </c>
       <c r="C76" t="n">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="D76" t="n">
         <v>9</v>
       </c>
       <c r="E76" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="77">
@@ -4532,13 +4532,13 @@
         <v>19</v>
       </c>
       <c r="C78" t="n">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="D78" t="n">
         <v>6</v>
       </c>
       <c r="E78" t="n">
-        <v>0.1666666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79">
@@ -4566,13 +4566,13 @@
         <v>19.5</v>
       </c>
       <c r="C80" t="n">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="D80" t="n">
         <v>6</v>
       </c>
       <c r="E80" t="n">
-        <v>0.1666666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81">
@@ -4583,13 +4583,13 @@
         <v>19.75</v>
       </c>
       <c r="C81" t="n">
-        <v>54</v>
+        <v>12</v>
       </c>
       <c r="D81" t="n">
         <v>9</v>
       </c>
       <c r="E81" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="82">
@@ -4600,13 +4600,13 @@
         <v>20</v>
       </c>
       <c r="C82" t="n">
-        <v>54</v>
+        <v>12</v>
       </c>
       <c r="D82" t="n">
         <v>9</v>
       </c>
       <c r="E82" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="83">
@@ -4617,13 +4617,13 @@
         <v>20.25</v>
       </c>
       <c r="C83" t="n">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="D83" t="n">
         <v>6</v>
       </c>
       <c r="E83" t="n">
-        <v>0.1666666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="84">
@@ -4634,13 +4634,13 @@
         <v>20.5</v>
       </c>
       <c r="C84" t="n">
-        <v>54</v>
+        <v>12</v>
       </c>
       <c r="D84" t="n">
         <v>9</v>
       </c>
       <c r="E84" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="85">
@@ -4668,13 +4668,13 @@
         <v>21</v>
       </c>
       <c r="C86" t="n">
-        <v>60</v>
+        <v>12</v>
       </c>
       <c r="D86" t="n">
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.8333333333333334</v>
       </c>
     </row>
     <row r="87">
@@ -4702,13 +4702,13 @@
         <v>21.5</v>
       </c>
       <c r="C88" t="n">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="D88" t="n">
         <v>6</v>
       </c>
       <c r="E88" t="n">
-        <v>0.1666666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89">
@@ -4719,13 +4719,13 @@
         <v>21.75</v>
       </c>
       <c r="C89" t="n">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="D89" t="n">
         <v>6</v>
       </c>
       <c r="E89" t="n">
-        <v>0.1666666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="90">
@@ -4736,13 +4736,13 @@
         <v>22</v>
       </c>
       <c r="C90" t="n">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="D90" t="n">
         <v>3</v>
       </c>
       <c r="E90" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="91">
@@ -4753,13 +4753,13 @@
         <v>22.25</v>
       </c>
       <c r="C91" t="n">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="D91" t="n">
         <v>6</v>
       </c>
       <c r="E91" t="n">
-        <v>0.1666666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="92">
@@ -4770,13 +4770,13 @@
         <v>22.5</v>
       </c>
       <c r="C92" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D92" t="n">
         <v>2</v>
       </c>
       <c r="E92" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.3333333333333333</v>
       </c>
     </row>
     <row r="93">
@@ -4787,13 +4787,13 @@
         <v>22.75</v>
       </c>
       <c r="C93" t="n">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="D93" t="n">
         <v>4</v>
       </c>
       <c r="E93" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.6666666666666666</v>
       </c>
     </row>
     <row r="94">
@@ -4804,13 +4804,13 @@
         <v>23</v>
       </c>
       <c r="C94" t="n">
-        <v>54</v>
+        <v>12</v>
       </c>
       <c r="D94" t="n">
         <v>9</v>
       </c>
       <c r="E94" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="95">
@@ -4821,13 +4821,13 @@
         <v>23.25</v>
       </c>
       <c r="C95" t="n">
-        <v>48</v>
+        <v>12</v>
       </c>
       <c r="D95" t="n">
         <v>8</v>
       </c>
       <c r="E95" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.6666666666666666</v>
       </c>
     </row>
     <row r="96">
@@ -4838,13 +4838,13 @@
         <v>23.5</v>
       </c>
       <c r="C96" t="n">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="D96" t="n">
         <v>4</v>
       </c>
       <c r="E96" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.6666666666666666</v>
       </c>
     </row>
     <row r="97">
@@ -4855,13 +4855,13 @@
         <v>23.75</v>
       </c>
       <c r="C97" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="D97" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E97" t="n">
-        <v>0.1666666666666667</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>